<commit_message>
Revertidas notas para antes turnitin. Baixadas notas pos turnitin. Iniciado cômputo notas forms. Similaridade forms. Exportação df fim. Atualização notas pos turnitin.
</commit_message>
<xml_diff>
--- a/Materias/2S2020/PED_CE342/Turma_C/output/CE342_C.xlsx
+++ b/Materias/2S2020/PED_CE342/Turma_C/output/CE342_C.xlsx
@@ -750,7 +750,7 @@
         <v>76.11</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
@@ -844,7 +844,7 @@
         <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Chamada Turmas A e C
</commit_message>
<xml_diff>
--- a/Materias/2S2020/PED_CE342/Turma_C/output/CE342_C.xlsx
+++ b/Materias/2S2020/PED_CE342/Turma_C/output/CE342_C.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M37"/>
+  <dimension ref="A1:N37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -497,6 +497,11 @@
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
+          <t>2020-12-14</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
           <t>Email</t>
         </is>
       </c>
@@ -542,7 +547,10 @@
       <c r="L2" t="n">
         <v>0</v>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="M2" t="n">
+        <v>21.62</v>
+      </c>
+      <c r="N2" t="inlineStr">
         <is>
           <t>a230645@dac.unicamp.br</t>
         </is>
@@ -587,7 +595,10 @@
       <c r="L3" t="n">
         <v>0</v>
       </c>
-      <c r="M3" t="inlineStr">
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" t="inlineStr">
         <is>
           <t>b213549@dac.unicamp.br</t>
         </is>
@@ -634,7 +645,10 @@
       <c r="L4" t="n">
         <v>7</v>
       </c>
-      <c r="M4" t="inlineStr">
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" t="inlineStr">
         <is>
           <t>b257748@dac.unicamp.br</t>
         </is>
@@ -679,7 +693,10 @@
       <c r="L5" t="n">
         <v>7</v>
       </c>
-      <c r="M5" t="inlineStr">
+      <c r="M5" t="n">
+        <v>100</v>
+      </c>
+      <c r="N5" t="inlineStr">
         <is>
           <t>c232568@dac.unicamp.br</t>
         </is>
@@ -720,7 +737,10 @@
       <c r="L6" t="n">
         <v>0</v>
       </c>
-      <c r="M6" t="inlineStr">
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" t="inlineStr">
         <is>
           <t>d233566@dac.unicamp.br</t>
         </is>
@@ -767,7 +787,10 @@
       <c r="L7" t="n">
         <v>0</v>
       </c>
-      <c r="M7" t="inlineStr">
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" t="inlineStr">
         <is>
           <t>f215626@dac.unicamp.br</t>
         </is>
@@ -806,7 +829,10 @@
         <v>11.43</v>
       </c>
       <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr">
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" t="inlineStr">
         <is>
           <t>f91108@dac.unicamp.br</t>
         </is>
@@ -851,7 +877,10 @@
       <c r="L9" t="n">
         <v>7</v>
       </c>
-      <c r="M9" t="inlineStr">
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" t="inlineStr">
         <is>
           <t>f234311@dac.unicamp.br</t>
         </is>
@@ -898,7 +927,10 @@
       <c r="L10" t="n">
         <v>7</v>
       </c>
-      <c r="M10" t="inlineStr">
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" t="inlineStr">
         <is>
           <t>g216397@dac.unicamp.br</t>
         </is>
@@ -945,7 +977,10 @@
       <c r="L11" t="n">
         <v>0</v>
       </c>
-      <c r="M11" t="inlineStr">
+      <c r="M11" t="n">
+        <v>100</v>
+      </c>
+      <c r="N11" t="inlineStr">
         <is>
           <t>g197474@dac.unicamp.br</t>
         </is>
@@ -980,7 +1015,10 @@
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
-      <c r="M12" t="inlineStr">
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" t="inlineStr">
         <is>
           <t>g234982@dac.unicamp.br</t>
         </is>
@@ -1025,7 +1063,10 @@
       <c r="L13" t="n">
         <v>5</v>
       </c>
-      <c r="M13" t="inlineStr">
+      <c r="M13" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" t="inlineStr">
         <is>
           <t>g235042@dac.unicamp.br</t>
         </is>
@@ -1072,7 +1113,10 @@
       <c r="L14" t="n">
         <v>5</v>
       </c>
-      <c r="M14" t="inlineStr">
+      <c r="M14" t="n">
+        <v>0</v>
+      </c>
+      <c r="N14" t="inlineStr">
         <is>
           <t>g197724@dac.unicamp.br</t>
         </is>
@@ -1103,7 +1147,8 @@
       <c r="J15" t="inlineStr"/>
       <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr"/>
-      <c r="M15" t="inlineStr">
+      <c r="M15" t="inlineStr"/>
+      <c r="N15" t="inlineStr">
         <is>
           <t>g217350@dac.unicamp.br</t>
         </is>
@@ -1144,7 +1189,10 @@
       <c r="L16" t="n">
         <v>0</v>
       </c>
-      <c r="M16" t="inlineStr">
+      <c r="M16" t="n">
+        <v>0</v>
+      </c>
+      <c r="N16" t="inlineStr">
         <is>
           <t>g174154@dac.unicamp.br</t>
         </is>
@@ -1181,7 +1229,8 @@
       <c r="L17" t="n">
         <v>0</v>
       </c>
-      <c r="M17" t="inlineStr">
+      <c r="M17" t="inlineStr"/>
+      <c r="N17" t="inlineStr">
         <is>
           <t>j237534@dac.unicamp.br</t>
         </is>
@@ -1228,7 +1277,10 @@
       <c r="L18" t="n">
         <v>7</v>
       </c>
-      <c r="M18" t="inlineStr">
+      <c r="M18" t="n">
+        <v>0</v>
+      </c>
+      <c r="N18" t="inlineStr">
         <is>
           <t>j237856@dac.unicamp.br</t>
         </is>
@@ -1275,7 +1327,10 @@
       <c r="L19" t="n">
         <v>10</v>
       </c>
-      <c r="M19" t="inlineStr">
+      <c r="M19" t="n">
+        <v>59.46</v>
+      </c>
+      <c r="N19" t="inlineStr">
         <is>
           <t>j199967@dac.unicamp.br</t>
         </is>
@@ -1322,7 +1377,10 @@
       <c r="L20" t="n">
         <v>0</v>
       </c>
-      <c r="M20" t="inlineStr">
+      <c r="M20" t="n">
+        <v>0</v>
+      </c>
+      <c r="N20" t="inlineStr">
         <is>
           <t>l103034@dac.unicamp.br</t>
         </is>
@@ -1369,7 +1427,10 @@
       <c r="L21" t="n">
         <v>0</v>
       </c>
-      <c r="M21" t="inlineStr">
+      <c r="M21" t="n">
+        <v>0</v>
+      </c>
+      <c r="N21" t="inlineStr">
         <is>
           <t>l172577@dac.unicamp.br</t>
         </is>
@@ -1416,7 +1477,10 @@
       <c r="L22" t="n">
         <v>7</v>
       </c>
-      <c r="M22" t="inlineStr">
+      <c r="M22" t="n">
+        <v>0</v>
+      </c>
+      <c r="N22" t="inlineStr">
         <is>
           <t>m159866@dac.unicamp.br</t>
         </is>
@@ -1463,7 +1527,10 @@
       <c r="L23" t="n">
         <v>0</v>
       </c>
-      <c r="M23" t="inlineStr">
+      <c r="M23" t="n">
+        <v>0</v>
+      </c>
+      <c r="N23" t="inlineStr">
         <is>
           <t>m221896@dac.unicamp.br</t>
         </is>
@@ -1510,7 +1577,10 @@
       <c r="L24" t="n">
         <v>0</v>
       </c>
-      <c r="M24" t="inlineStr">
+      <c r="M24" t="n">
+        <v>0</v>
+      </c>
+      <c r="N24" t="inlineStr">
         <is>
           <t>m257876@dac.unicamp.br</t>
         </is>
@@ -1545,7 +1615,10 @@
       <c r="J25" t="inlineStr"/>
       <c r="K25" t="inlineStr"/>
       <c r="L25" t="inlineStr"/>
-      <c r="M25" t="inlineStr">
+      <c r="M25" t="n">
+        <v>0</v>
+      </c>
+      <c r="N25" t="inlineStr">
         <is>
           <t>m242087@dac.unicamp.br</t>
         </is>
@@ -1582,7 +1655,10 @@
       <c r="L26" t="n">
         <v>0</v>
       </c>
-      <c r="M26" t="inlineStr">
+      <c r="M26" t="n">
+        <v>0</v>
+      </c>
+      <c r="N26" t="inlineStr">
         <is>
           <t>n242328@dac.unicamp.br</t>
         </is>
@@ -1629,7 +1705,10 @@
       <c r="L27" t="n">
         <v>0</v>
       </c>
-      <c r="M27" t="inlineStr">
+      <c r="M27" t="n">
+        <v>0</v>
+      </c>
+      <c r="N27" t="inlineStr">
         <is>
           <t>p147614@dac.unicamp.br</t>
         </is>
@@ -1658,7 +1737,8 @@
       <c r="J28" t="inlineStr"/>
       <c r="K28" t="inlineStr"/>
       <c r="L28" t="inlineStr"/>
-      <c r="M28" t="inlineStr">
+      <c r="M28" t="inlineStr"/>
+      <c r="N28" t="inlineStr">
         <is>
           <t>r176104@dac.unicamp.br</t>
         </is>
@@ -1693,7 +1773,8 @@
       <c r="L29" t="n">
         <v>0</v>
       </c>
-      <c r="M29" t="inlineStr">
+      <c r="M29" t="inlineStr"/>
+      <c r="N29" t="inlineStr">
         <is>
           <t>r205149@dac.unicamp.br</t>
         </is>
@@ -1738,7 +1819,10 @@
       <c r="L30" t="n">
         <v>0</v>
       </c>
-      <c r="M30" t="inlineStr">
+      <c r="M30" t="n">
+        <v>0</v>
+      </c>
+      <c r="N30" t="inlineStr">
         <is>
           <t>r205151@dac.unicamp.br</t>
         </is>
@@ -1781,9 +1865,12 @@
         <v>85.70999999999999</v>
       </c>
       <c r="L31" t="n">
-        <v>7</v>
-      </c>
-      <c r="M31" t="inlineStr">
+        <v>0</v>
+      </c>
+      <c r="M31" t="n">
+        <v>0</v>
+      </c>
+      <c r="N31" t="inlineStr">
         <is>
           <t>s244207@dac.unicamp.br</t>
         </is>
@@ -1830,7 +1917,10 @@
       <c r="L32" t="n">
         <v>10</v>
       </c>
-      <c r="M32" t="inlineStr">
+      <c r="M32" t="n">
+        <v>0</v>
+      </c>
+      <c r="N32" t="inlineStr">
         <is>
           <t>t158425@dac.unicamp.br</t>
         </is>
@@ -1877,7 +1967,10 @@
       <c r="L33" t="n">
         <v>7</v>
       </c>
-      <c r="M33" t="inlineStr">
+      <c r="M33" t="n">
+        <v>0</v>
+      </c>
+      <c r="N33" t="inlineStr">
         <is>
           <t>t257932@dac.unicamp.br</t>
         </is>
@@ -1918,7 +2011,10 @@
       <c r="L34" t="n">
         <v>10</v>
       </c>
-      <c r="M34" t="inlineStr">
+      <c r="M34" t="n">
+        <v>0</v>
+      </c>
+      <c r="N34" t="inlineStr">
         <is>
           <t>v177964@dac.unicamp.br</t>
         </is>
@@ -1965,7 +2061,10 @@
       <c r="L35" t="n">
         <v>7</v>
       </c>
-      <c r="M35" t="inlineStr">
+      <c r="M35" t="n">
+        <v>0</v>
+      </c>
+      <c r="N35" t="inlineStr">
         <is>
           <t>v245099@dac.unicamp.br</t>
         </is>
@@ -2012,7 +2111,10 @@
       <c r="L36" t="n">
         <v>3</v>
       </c>
-      <c r="M36" t="inlineStr">
+      <c r="M36" t="n">
+        <v>83.78</v>
+      </c>
+      <c r="N36" t="inlineStr">
         <is>
           <t>v206806@dac.unicamp.br</t>
         </is>
@@ -2051,7 +2153,10 @@
       <c r="L37" t="n">
         <v>0</v>
       </c>
-      <c r="M37" t="inlineStr">
+      <c r="M37" t="n">
+        <v>13.51</v>
+      </c>
+      <c r="N37" t="inlineStr">
         <is>
           <t>w225851@dac.unicamp.br</t>
         </is>

</xml_diff>

<commit_message>
SFC grammar fixes. Turma C rjust added (RA < 010)
</commit_message>
<xml_diff>
--- a/Materias/2S2020/PED_CE342/Turma_C/output/CE342_C.xlsx
+++ b/Materias/2S2020/PED_CE342/Turma_C/output/CE342_C.xlsx
@@ -799,7 +799,7 @@
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>91108</t>
+          <t>091108</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -807,7 +807,9 @@
           <t>felipe eboli sotorilli</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr"/>
+      <c r="C8" t="n">
+        <v>50</v>
+      </c>
       <c r="D8" t="n">
         <v>1.79</v>
       </c>
@@ -817,24 +819,30 @@
       <c r="F8" t="n">
         <v>77.88</v>
       </c>
-      <c r="G8" t="inlineStr"/>
+      <c r="G8" t="n">
+        <v>7</v>
+      </c>
       <c r="H8" t="n">
         <v>29.17</v>
       </c>
       <c r="I8" t="n">
         <v>76.47</v>
       </c>
-      <c r="J8" t="inlineStr"/>
+      <c r="J8" t="n">
+        <v>5</v>
+      </c>
       <c r="K8" t="n">
         <v>11.43</v>
       </c>
-      <c r="L8" t="inlineStr"/>
+      <c r="L8" t="n">
+        <v>7</v>
+      </c>
       <c r="M8" t="n">
         <v>0</v>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>f91108@dac.unicamp.br</t>
+          <t>f091108@dac.unicamp.br</t>
         </is>
       </c>
     </row>

</xml_diff>